<commit_message>
Read quarterly S&L tax  revenue
Replace annual  S&L tax revenue with quarterly numbers
</commit_message>
<xml_diff>
--- a/results/12-2020/fim.xlsx
+++ b/results/12-2020/fim.xlsx
@@ -82697,7 +82697,7 @@
         <v>1475.257314660539</v>
       </c>
       <c r="AM205">
-        <v>1490.738044351792</v>
+        <v>1490.738044351791</v>
       </c>
       <c r="AN205">
         <v>5170.12504575753</v>
@@ -82763,19 +82763,19 @@
         <v>-517.1226500000001</v>
       </c>
       <c r="BI205">
-        <v>509.4987103135083</v>
+        <v>509.4987103135082</v>
       </c>
       <c r="BJ205">
         <v>20.60847807035016</v>
       </c>
       <c r="BK205">
-        <v>1343.93802782536</v>
+        <v>1343.938027825359</v>
       </c>
       <c r="BL205">
-        <v>1874.136436317675</v>
+        <v>1874.136436317674</v>
       </c>
       <c r="BM205">
-        <v>80.70144256430407</v>
+        <v>80.70144256430406</v>
       </c>
       <c r="BN205">
         <v>0.6019649465167092</v>
@@ -82889,10 +82889,10 @@
         <v>-594.7479736244353</v>
       </c>
       <c r="CZ205">
-        <v>28.15969731005157</v>
+        <v>28.15969731005111</v>
       </c>
       <c r="DA205">
-        <v>1.210582933674772</v>
+        <v>1.210582933674758</v>
       </c>
       <c r="DB205">
         <v>0</v>
@@ -82943,7 +82943,7 @@
         <v>0.9396232617285506</v>
       </c>
       <c r="DR205">
-        <v>-0.639703225278745</v>
+        <v>-0.6397032252787445</v>
       </c>
       <c r="DS205">
         <v>-7.100797520415836</v>
@@ -82952,7 +82952,7 @@
         <v>-3.718441421380831</v>
       </c>
       <c r="DU205">
-        <v>-3.382356099035128</v>
+        <v>-3.382356099035074</v>
       </c>
       <c r="DV205">
         <v>4.729087960674262</v>
@@ -82967,13 +82967,13 @@
         <v>-166.1340003649827</v>
       </c>
       <c r="DZ205">
-        <v>-217.7186087072994</v>
+        <v>-217.7186087072993</v>
       </c>
       <c r="EA205">
         <v>45.26665974128039</v>
       </c>
       <c r="EB205">
-        <v>-4.116227813968822</v>
+        <v>-4.11622781396882</v>
       </c>
       <c r="EC205">
         <v>0.8558197435618375</v>
@@ -83002,22 +83002,22 @@
         <v>44286</v>
       </c>
       <c r="B206">
-        <v>-2.441210859714101</v>
+        <v>3.274442939439371</v>
       </c>
       <c r="C206">
-        <v>3.056954023466782</v>
+        <v>4.485867473255149</v>
       </c>
       <c r="D206">
-        <v>0.1642490337702971</v>
+        <v>-3.368956404567739</v>
       </c>
       <c r="E206">
-        <v>-0.4326965979299264</v>
+        <v>3.100508840408109</v>
       </c>
       <c r="F206">
-        <v>-2.172763295554471</v>
+        <v>3.542890503599001</v>
       </c>
       <c r="G206">
-        <v>-0.1137921146241706</v>
+        <v>0.2531305103579604</v>
       </c>
       <c r="I206">
         <v>21942.91648059992</v>
@@ -83050,7 +83050,7 @@
         <v>523.17084771922</v>
       </c>
       <c r="S206">
-        <v>282.1409954476429</v>
+        <v>472.8009954476429</v>
       </c>
       <c r="T206">
         <v>74.70668003712791</v>
@@ -83101,7 +83101,7 @@
         <v>3703.464861448391</v>
       </c>
       <c r="AJ206">
-        <v>1955.568889579091</v>
+        <v>3238.368889579091</v>
       </c>
       <c r="AK206">
         <v>2219.828214992802</v>
@@ -83110,16 +83110,16 @@
         <v>1495.447941076645</v>
       </c>
       <c r="AM206">
-        <v>1515.127156803014</v>
+        <v>1515.127156803013</v>
       </c>
       <c r="AN206">
-        <v>5230.496045858525</v>
+        <v>5230.496045858524</v>
       </c>
       <c r="AO206">
-        <v>307.6031794471427</v>
+        <v>307.6031794471426</v>
       </c>
       <c r="AP206">
-        <v>100.8542546295093</v>
+        <v>500.8542546295093</v>
       </c>
       <c r="AQ206">
         <v>0</v>
@@ -83137,7 +83137,7 @@
         <v>0</v>
       </c>
       <c r="AV206">
-        <v>2494.184346204091</v>
+        <v>3776.984346204091</v>
       </c>
       <c r="AW206">
         <v>1701.879512646469</v>
@@ -83155,7 +83155,7 @@
         <v>225.5633104395484</v>
       </c>
       <c r="BB206">
-        <v>100.2502499999998</v>
+        <v>500.2502499999998</v>
       </c>
       <c r="BC206">
         <v>220.8917747488439</v>
@@ -83176,7 +83176,7 @@
         <v>-538.6154566249999</v>
       </c>
       <c r="BI206">
-        <v>517.948702346333</v>
+        <v>517.9487023463329</v>
       </c>
       <c r="BJ206">
         <v>20.95026789626738</v>
@@ -83188,7 +83188,7 @@
         <v>1905.218826978813</v>
       </c>
       <c r="BM206">
-        <v>82.03986900759421</v>
+        <v>82.03986900759419</v>
       </c>
       <c r="BN206">
         <v>0.6040046295094899</v>
@@ -83209,13 +83209,13 @@
         <v>53.36225624681128</v>
       </c>
       <c r="BT206">
-        <v>440.9267533528007</v>
+        <v>1723.726753352801</v>
       </c>
       <c r="BU206">
-        <v>-1120.543773676931</v>
+        <v>-720.5437736769309</v>
       </c>
       <c r="BV206">
-        <v>68.61464764872966</v>
+        <v>259.2746476487297</v>
       </c>
       <c r="BX206">
         <v>244</v>
@@ -83233,7 +83233,7 @@
         <v>-0.176451333688259</v>
       </c>
       <c r="CC206">
-        <v>-0.3371659659437569</v>
+        <v>3.196039472394279</v>
       </c>
       <c r="CD206">
         <v>-0.003534401514799262</v>
@@ -83242,7 +83242,7 @@
         <v>-0.09199623047137026</v>
       </c>
       <c r="CF206">
-        <v>-0.3407003674585561</v>
+        <v>3.19250507087948</v>
       </c>
       <c r="CG206">
         <v>-0.176451333688259</v>
@@ -83251,19 +83251,19 @@
         <v>-0.2684475641596293</v>
       </c>
       <c r="CI206">
-        <v>-284.8124373989151</v>
+        <v>115.1875626010849</v>
       </c>
       <c r="CJ206">
         <v>13.02143192736162</v>
       </c>
       <c r="CK206">
-        <v>-74.67509550372642</v>
+        <v>1208.124904496274</v>
       </c>
       <c r="CL206">
-        <v>31.62146729067445</v>
+        <v>31.62146729067354</v>
       </c>
       <c r="CM206">
-        <v>9.823373288389575</v>
+        <v>9.823373288389519</v>
       </c>
       <c r="CN206">
         <v>0</v>
@@ -83272,13 +83272,13 @@
         <v>-95.67840566666672</v>
       </c>
       <c r="CP206">
-        <v>-284.8111297332795</v>
+        <v>115.1888702667205</v>
       </c>
       <c r="CQ206">
         <v>12.19845212836162</v>
       </c>
       <c r="CR206">
-        <v>-76.50271093158335</v>
+        <v>1206.297289068417</v>
       </c>
       <c r="CS206">
         <v>10.96059380563247</v>
@@ -83323,10 +83323,10 @@
         <v>-3.748618644962366</v>
       </c>
       <c r="DG206">
-        <v>-139.3283210077842</v>
+        <v>149.3016789922159</v>
       </c>
       <c r="DH206">
-        <v>42.76731354412304</v>
+        <v>331.3973135441231</v>
       </c>
       <c r="DI206">
         <v>-182.7973550515025</v>
@@ -83350,64 +83350,64 @@
         <v>-1.528274372812393</v>
       </c>
       <c r="DP206">
-        <v>-1.289974539117559</v>
+        <v>-1.289974539117557</v>
       </c>
       <c r="DQ206">
         <v>-0.6002654852329177</v>
       </c>
       <c r="DR206">
-        <v>-0.6897090538846381</v>
+        <v>-0.6897090538846375</v>
       </c>
       <c r="DS206">
-        <v>3.134985910807446</v>
+        <v>3.134985910807555</v>
       </c>
       <c r="DT206">
         <v>6.035944186472268</v>
       </c>
       <c r="DU206">
-        <v>-2.900958275664866</v>
+        <v>-2.900958275664812</v>
       </c>
       <c r="DV206">
-        <v>-6.140487710912628</v>
+        <v>13.65951228908737</v>
       </c>
       <c r="DW206">
-        <v>-6.138643359355542</v>
+        <v>13.66135664064446</v>
       </c>
       <c r="DX206">
         <v>-0.001844351557086037</v>
       </c>
       <c r="DY206">
-        <v>-117.2473713063445</v>
+        <v>191.1826286936556</v>
       </c>
       <c r="DZ206">
-        <v>-190.1384853775715</v>
+        <v>-190.1384853775714</v>
       </c>
       <c r="EA206">
-        <v>72.1893935716316</v>
+        <v>380.6193935716317</v>
       </c>
       <c r="EB206">
-        <v>-3.523541018427529</v>
+        <v>-3.523541018427528</v>
       </c>
       <c r="EC206">
-        <v>1.337773827533901</v>
+        <v>7.053427626687371</v>
       </c>
       <c r="ED206">
         <v>0.4887933070952966</v>
       </c>
       <c r="EE206">
-        <v>-2.581955216087331</v>
+        <v>2.766775958084007</v>
       </c>
       <c r="EF206">
-        <v>0.05809582119573056</v>
+        <v>0.05809582119573258</v>
       </c>
       <c r="EG206">
-        <v>-0.02390509313399644</v>
+        <v>-0.0239050931339964</v>
       </c>
       <c r="EH206">
         <v>-3.417850074322673e-05</v>
       </c>
       <c r="EI206">
-        <v>-0.1137579361234274</v>
+        <v>0.2531646888587037</v>
       </c>
     </row>
     <row r="207">
@@ -83415,22 +83415,22 @@
         <v>44377</v>
       </c>
       <c r="B207">
-        <v>-3.259373598073963</v>
+        <v>-2.987287850227718</v>
       </c>
       <c r="C207">
-        <v>-1.330333772243113</v>
+        <v>0.1666011145068151</v>
       </c>
       <c r="D207">
-        <v>0.2541332789429268</v>
+        <v>0.2868626796071934</v>
       </c>
       <c r="E207">
-        <v>-0.6710165752478724</v>
+        <v>-0.7037459759121391</v>
       </c>
       <c r="F207">
-        <v>-2.842490301769017</v>
+        <v>-2.570404553922772</v>
       </c>
       <c r="G207">
-        <v>-0.08831959063148859</v>
+        <v>0.2208540867683731</v>
       </c>
       <c r="I207">
         <v>22291.8404896825</v>
@@ -83463,7 +83463,7 @@
         <v>541.72027157883</v>
       </c>
       <c r="S207">
-        <v>255.0224339220724</v>
+        <v>445.6824339220724</v>
       </c>
       <c r="T207">
         <v>75.04939368825832</v>
@@ -83526,13 +83526,13 @@
         <v>1538.952154407404</v>
       </c>
       <c r="AN207">
-        <v>5290.080381569621</v>
+        <v>5290.08038156962</v>
       </c>
       <c r="AO207">
         <v>319.0393868682636</v>
       </c>
       <c r="AP207">
-        <v>100.8564375574148</v>
+        <v>500.8564375574148</v>
       </c>
       <c r="AQ207">
         <v>0</v>
@@ -83568,7 +83568,7 @@
         <v>235.6949656593226</v>
       </c>
       <c r="BB207">
-        <v>100.2502500000001</v>
+        <v>500.2502500000001</v>
       </c>
       <c r="BC207">
         <v>228.723662123266</v>
@@ -83589,7 +83589,7 @@
         <v>-556.1119952665625</v>
       </c>
       <c r="BI207">
-        <v>526.1848334860374</v>
+        <v>526.1848334860373</v>
       </c>
       <c r="BJ207">
         <v>21.28340736166992</v>
@@ -83601,7 +83601,7 @@
         <v>1935.514553250053</v>
       </c>
       <c r="BM207">
-        <v>83.34442120894099</v>
+        <v>83.34442120894097</v>
       </c>
       <c r="BN207">
         <v>0.6061875574147406</v>
@@ -83625,10 +83625,10 @@
         <v>517.2278108710334</v>
       </c>
       <c r="BU207">
-        <v>-1124.95583479476</v>
+        <v>-724.95583479476</v>
       </c>
       <c r="BV207">
-        <v>56.66594358351176</v>
+        <v>247.3259435835118</v>
       </c>
       <c r="BX207">
         <v>152</v>
@@ -83646,7 +83646,7 @@
         <v>-0.295224586287391</v>
       </c>
       <c r="CC207">
-        <v>-0.5427808076397411</v>
+        <v>-0.5755102083040079</v>
       </c>
       <c r="CD207">
         <v>-0.006577057590576529</v>
@@ -83655,7 +83655,7 @@
         <v>-0.1216587100175547</v>
       </c>
       <c r="CF207">
-        <v>-0.5493578652303177</v>
+        <v>-0.5820872658945844</v>
       </c>
       <c r="CG207">
         <v>-0.295224586287391</v>
@@ -83664,19 +83664,19 @@
         <v>-0.4168832963049456</v>
       </c>
       <c r="CI207">
-        <v>-0.7087353870145989</v>
+        <v>-3.528322195847522</v>
       </c>
       <c r="CJ207">
         <v>4.714920809861496</v>
       </c>
       <c r="CK207">
-        <v>-73.88132971463256</v>
+        <v>-1365.72374461056</v>
       </c>
       <c r="CL207">
         <v>22.71474157470857</v>
       </c>
       <c r="CM207">
-        <v>9.267922753310415</v>
+        <v>9.267922753310472</v>
       </c>
       <c r="CN207">
         <v>0</v>
@@ -83685,13 +83685,13 @@
         <v>-93.71994795338804</v>
       </c>
       <c r="CP207">
-        <v>-0.7066607062052555</v>
+        <v>-3.526247515038108</v>
       </c>
       <c r="CQ207">
         <v>6.041035998057851</v>
       </c>
       <c r="CR207">
-        <v>-76.60441168572788</v>
+        <v>-1368.446826581655</v>
       </c>
       <c r="CS207">
         <v>5.848839984691949</v>
@@ -83715,7 +83715,7 @@
         <v>2.723081971095553</v>
       </c>
       <c r="CZ207">
-        <v>16.86590159001662</v>
+        <v>16.86590159001685</v>
       </c>
       <c r="DA207">
         <v>0.7262558702163062</v>
@@ -83736,10 +83736,10 @@
         <v>5.993578954459299</v>
       </c>
       <c r="DG207">
-        <v>-166.78937999811</v>
+        <v>-168.8239233496935</v>
       </c>
       <c r="DH207">
-        <v>11.3957321077464</v>
+        <v>9.361188756162846</v>
       </c>
       <c r="DI207">
         <v>-173.1076892043021</v>
@@ -83769,49 +83769,49 @@
         <v>-0.4147559027844939</v>
       </c>
       <c r="DR207">
-        <v>-0.5524434137781412</v>
+        <v>-0.5524434137781408</v>
       </c>
       <c r="DS207">
-        <v>3.473187065253112</v>
+        <v>3.473187065253221</v>
       </c>
       <c r="DT207">
         <v>4.576855784762992</v>
       </c>
       <c r="DU207">
-        <v>-1.103668719509893</v>
+        <v>-1.103668719509892</v>
       </c>
       <c r="DV207">
-        <v>-4.844973502068824</v>
+        <v>12.11545695089395</v>
       </c>
       <c r="DW207">
-        <v>-4.843273033817867</v>
+        <v>12.11715741914491</v>
       </c>
       <c r="DX207">
         <v>-0.001700468250960165</v>
       </c>
       <c r="DY207">
-        <v>-155.931318221582</v>
+        <v>-141.0054311202027</v>
       </c>
       <c r="DZ207">
         <v>-168.7719228513818</v>
       </c>
       <c r="EA207">
-        <v>17.91802753135404</v>
+        <v>32.84391463273327</v>
       </c>
       <c r="EB207">
         <v>-3.076563190687906</v>
       </c>
       <c r="EC207">
-        <v>0.3266298269365542</v>
+        <v>0.5987155747827977</v>
       </c>
       <c r="ED207">
         <v>0.2405705283812016</v>
       </c>
       <c r="EE207">
-        <v>-3.040423184321392</v>
+        <v>-3.077511113875011</v>
       </c>
       <c r="EF207">
-        <v>0.06331313466601053</v>
+        <v>0.06331313466601252</v>
       </c>
       <c r="EG207">
         <v>-0.01763118986334844</v>
@@ -83820,7 +83820,7 @@
         <v>-3.099803533342663e-05</v>
       </c>
       <c r="EI207">
-        <v>-0.08828859259615522</v>
+        <v>0.2208850848037065</v>
       </c>
     </row>
     <row r="208">
@@ -83828,22 +83828,22 @@
         <v>44469</v>
       </c>
       <c r="B208">
-        <v>-3.173445527074861</v>
+        <v>-2.924166013534065</v>
       </c>
       <c r="C208">
-        <v>-3.04545543301559</v>
+        <v>-1.486200667880462</v>
       </c>
       <c r="D208">
-        <v>-0.1580530711298793</v>
+        <v>-0.1256411816786448</v>
       </c>
       <c r="E208">
-        <v>-0.117563065932944</v>
+        <v>-0.1499749553841785</v>
       </c>
       <c r="F208">
-        <v>-2.897829390012038</v>
+        <v>-2.648549876471242</v>
       </c>
       <c r="G208">
-        <v>-0.04745662604278882</v>
+        <v>0.2383302966107768</v>
       </c>
       <c r="I208">
         <v>22664.78462982512</v>
@@ -83876,7 +83876,7 @@
         <v>560.2696954384398</v>
       </c>
       <c r="S208">
-        <v>256.0549761349776</v>
+        <v>446.7149761349775</v>
       </c>
       <c r="T208">
         <v>75.45085825101107</v>
@@ -83945,7 +83945,7 @@
         <v>330.5654004191876</v>
       </c>
       <c r="AP208">
-        <v>100.8587948704311</v>
+        <v>500.8587948704311</v>
       </c>
       <c r="AQ208">
         <v>0</v>
@@ -83981,7 +83981,7 @@
         <v>245.8266208790969</v>
       </c>
       <c r="BB208">
-        <v>100.2502500000003</v>
+        <v>500.2502500000003</v>
       </c>
       <c r="BC208">
         <v>236.5555494976879</v>
@@ -84002,7 +84002,7 @@
         <v>-559.1125552428954</v>
       </c>
       <c r="BI208">
-        <v>534.9879446679679</v>
+        <v>534.9879446679678</v>
       </c>
       <c r="BJ208">
         <v>21.6394803409951</v>
@@ -84038,10 +84038,10 @@
         <v>495.3425409759989</v>
       </c>
       <c r="BU208">
-        <v>-1129.720357285768</v>
+        <v>-729.7203572857679</v>
       </c>
       <c r="BV208">
-        <v>72.28898901689669</v>
+        <v>262.9489890168967</v>
       </c>
       <c r="BX208">
         <v>44</v>
@@ -84059,7 +84059,7 @@
         <v>-0.1884332344784254</v>
       </c>
       <c r="CC208">
-        <v>-0.0248256825878863</v>
+        <v>-0.05723757203912079</v>
       </c>
       <c r="CD208">
         <v>-0.005554480760659826</v>
@@ -84068,7 +84068,7 @@
         <v>-0.0871829025843979</v>
       </c>
       <c r="CF208">
-        <v>-0.03038016334854612</v>
+        <v>-0.06279205279978062</v>
       </c>
       <c r="CG208">
         <v>-0.1884332344784254</v>
@@ -84077,7 +84077,7 @@
         <v>-0.2756161370628233</v>
       </c>
       <c r="CI208">
-        <v>-0.7753142264103019</v>
+        <v>-3.859585526331614</v>
       </c>
       <c r="CJ208">
         <v>-1.614949901188083</v>
@@ -84086,7 +84086,7 @@
         <v>-78.00748108314201</v>
       </c>
       <c r="CL208">
-        <v>20.87980333247197</v>
+        <v>20.87980333247287</v>
       </c>
       <c r="CM208">
         <v>9.06600348976832</v>
@@ -84098,7 +84098,7 @@
         <v>-109.1720230939701</v>
       </c>
       <c r="CP208">
-        <v>-0.7729974222121143</v>
+        <v>-3.857268722133426</v>
       </c>
       <c r="CQ208">
         <v>-0.1643476347387605</v>
@@ -84128,10 +84128,10 @@
         <v>1.626710533015057</v>
       </c>
       <c r="CZ208">
-        <v>17.45717166257418</v>
+        <v>17.45717166257441</v>
       </c>
       <c r="DA208">
-        <v>0.7517163152915458</v>
+        <v>0.75171631529156</v>
       </c>
       <c r="DB208">
         <v>0</v>
@@ -84149,10 +84149,10 @@
         <v>-4.933260291017048</v>
       </c>
       <c r="DG208">
-        <v>-166.0252511381175</v>
+        <v>-168.0597944897011</v>
       </c>
       <c r="DH208">
-        <v>-24.61955303883649</v>
+        <v>-26.65409639042004</v>
       </c>
       <c r="DI208">
         <v>-140.8212576788797</v>
@@ -84185,46 +84185,46 @@
         <v>-0.5513368906233805</v>
       </c>
       <c r="DS208">
-        <v>0.3683455122886699</v>
+        <v>0.3683455122886144</v>
       </c>
       <c r="DT208">
         <v>4.526138305143604</v>
       </c>
       <c r="DU208">
-        <v>-4.157792792855017</v>
+        <v>-4.157792792855044</v>
       </c>
       <c r="DV208">
-        <v>-2.644738844810903</v>
+        <v>13.28205238976538</v>
       </c>
       <c r="DW208">
-        <v>-2.643142230887218</v>
+        <v>13.28364900368908</v>
       </c>
       <c r="DX208">
         <v>-0.001596613923682332</v>
       </c>
       <c r="DY208">
-        <v>-161.4948763211557</v>
+        <v>-147.6026284381631</v>
       </c>
       <c r="DZ208">
-        <v>-150.4652442672988</v>
+        <v>-150.4652442672989</v>
       </c>
       <c r="EA208">
-        <v>-10.44519163345563</v>
+        <v>3.447056249537128</v>
       </c>
       <c r="EB208">
         <v>-2.69991604034561</v>
       </c>
       <c r="EC208">
-        <v>-0.187426276233944</v>
+        <v>0.06185323730685323</v>
       </c>
       <c r="ED208">
         <v>0.1398026042248747</v>
       </c>
       <c r="EE208">
-        <v>-2.979121463119391</v>
+        <v>-3.015628872232159</v>
       </c>
       <c r="EF208">
-        <v>0.006609512793870096</v>
+        <v>0.006609512793869101</v>
       </c>
       <c r="EG208">
         <v>-0.01766341786860341</v>
@@ -84233,7 +84233,7 @@
         <v>-2.864929747584198e-05</v>
       </c>
       <c r="EI208">
-        <v>-0.04742797674531295</v>
+        <v>0.2383589459082528</v>
       </c>
     </row>
     <row r="209">
@@ -84241,22 +84241,22 @@
         <v>44561</v>
       </c>
       <c r="B209">
-        <v>-2.475255620977485</v>
+        <v>-2.597578075119432</v>
       </c>
       <c r="C209">
-        <v>-2.837321401460102</v>
+        <v>-1.308647249860461</v>
       </c>
       <c r="D209">
-        <v>0.03569302105791163</v>
+        <v>3.433091938529865</v>
       </c>
       <c r="E209">
-        <v>-0.1571543546386199</v>
+        <v>-3.554553272110574</v>
       </c>
       <c r="F209">
-        <v>-2.353794287396777</v>
+        <v>-2.476116741538723</v>
       </c>
       <c r="G209">
-        <v>-0.01524588712786182</v>
+        <v>-0.1016616536958829</v>
       </c>
       <c r="I209">
         <v>22914.57292255905</v>
@@ -84349,7 +84349,7 @@
         <v>1559.347249516656</v>
       </c>
       <c r="AM209">
-        <v>1583.583825651546</v>
+        <v>1583.583825651547</v>
       </c>
       <c r="AN209">
         <v>5421.993918611828</v>
@@ -84415,7 +84415,7 @@
         <v>-563.635899407217</v>
       </c>
       <c r="BI209">
-        <v>540.8840397562044</v>
+        <v>540.8840397562042</v>
       </c>
       <c r="BJ209">
         <v>21.87796876867306</v>
@@ -84427,7 +84427,7 @@
         <v>1989.584009164711</v>
       </c>
       <c r="BM209">
-        <v>85.67268451273401</v>
+        <v>85.67268451273404</v>
       </c>
       <c r="BN209">
         <v>0.6110859106172505</v>
@@ -84472,7 +84472,7 @@
         <v>-0.09025519427828409</v>
       </c>
       <c r="CC209">
-        <v>-0.1232946583972288</v>
+        <v>-3.520693575869183</v>
       </c>
       <c r="CD209">
         <v>-0.002653556938966896</v>
@@ -84481,16 +84481,16 @@
         <v>-0.03120613930242417</v>
       </c>
       <c r="CF209">
-        <v>-0.1259482153361957</v>
+        <v>-3.52334713280815</v>
       </c>
       <c r="CG209">
         <v>-0.09025519427828409</v>
       </c>
       <c r="CH209">
-        <v>-0.1214613335807083</v>
+        <v>-0.1214613335807084</v>
       </c>
       <c r="CI209">
-        <v>-0.7637870421930444</v>
+        <v>-403.802998777228</v>
       </c>
       <c r="CJ209">
         <v>23.90952447025347</v>
@@ -84502,7 +84502,7 @@
         <v>29.58087024093402</v>
       </c>
       <c r="CM209">
-        <v>41.37209537120367</v>
+        <v>41.37209537120373</v>
       </c>
       <c r="CN209">
         <v>0</v>
@@ -84511,7 +84511,7 @@
         <v>-0.3343132908538493</v>
       </c>
       <c r="CP209">
-        <v>-0.7617043406007014</v>
+        <v>-403.8009160756357</v>
       </c>
       <c r="CQ209">
         <v>25.33893420835716</v>
@@ -84544,7 +84544,7 @@
         <v>6.73602384546075</v>
       </c>
       <c r="DA209">
-        <v>0.2900572396662824</v>
+        <v>0.2900572396663108</v>
       </c>
       <c r="DB209">
         <v>0</v>
@@ -84562,10 +84562,10 @@
         <v>-0.7612081635936206</v>
       </c>
       <c r="DG209">
-        <v>-138.1616407511809</v>
+        <v>-140.1961841027644</v>
       </c>
       <c r="DH209">
-        <v>-128.2285440932863</v>
+        <v>-130.2630874448699</v>
       </c>
       <c r="DI209">
         <v>-11.20657095841259</v>
@@ -84589,64 +84589,64 @@
         <v>-0.7600972160279014</v>
       </c>
       <c r="DP209">
-        <v>-1.708819277203788</v>
+        <v>-1.70881927720379</v>
       </c>
       <c r="DQ209">
         <v>-1.177539698063183</v>
       </c>
       <c r="DR209">
-        <v>-0.5312795791406006</v>
+        <v>-0.5312795791406015</v>
       </c>
       <c r="DS209">
-        <v>-1.643238211822773</v>
+        <v>-1.643238211822827</v>
       </c>
       <c r="DT209">
         <v>3.221233610117506</v>
       </c>
       <c r="DU209">
-        <v>-4.864471821940293</v>
+        <v>-4.864471821940306</v>
       </c>
       <c r="DV209">
-        <v>-0.8638618706090277</v>
+        <v>-5.760348715322626</v>
       </c>
       <c r="DW209">
-        <v>-0.8623647126284111</v>
+        <v>-5.758851557342008</v>
       </c>
       <c r="DX209">
         <v>-0.001497157980611642</v>
       </c>
       <c r="DY209">
-        <v>-133.3706014669016</v>
+        <v>-140.3016316631988</v>
       </c>
       <c r="DZ209">
-        <v>-17.36502768106772</v>
+        <v>-17.36502768106773</v>
       </c>
       <c r="EA209">
-        <v>-117.2790480863519</v>
+        <v>-124.2100782826491</v>
       </c>
       <c r="EB209">
-        <v>-0.3064671112421104</v>
+        <v>-0.3064671112421106</v>
       </c>
       <c r="EC209">
-        <v>-2.069802118163905</v>
+        <v>-2.192124572305851</v>
       </c>
       <c r="ED209">
         <v>0.1589595275846998</v>
       </c>
       <c r="EE209">
-        <v>-2.438349060142769</v>
+        <v>-2.474255747716694</v>
       </c>
       <c r="EF209">
-        <v>-0.02900072934574278</v>
+        <v>-0.02900072934574374</v>
       </c>
       <c r="EG209">
-        <v>-0.03015813836510254</v>
+        <v>-0.03015813836510257</v>
       </c>
       <c r="EH209">
         <v>-2.642262885024721e-05</v>
       </c>
       <c r="EI209">
-        <v>-0.01521946449901148</v>
+        <v>-0.1016352310670325</v>
       </c>
     </row>
     <row r="210">
@@ -84654,10 +84654,10 @@
         <v>44651</v>
       </c>
       <c r="B210">
-        <v>-1.240773270103016</v>
+        <v>-6.368117040881671</v>
       </c>
       <c r="C210">
-        <v>-2.537212004057331</v>
+        <v>-3.719287244940721</v>
       </c>
       <c r="D210">
         <v>0.09133680375806208</v>
@@ -84666,10 +84666,10 @@
         <v>-0.148166807756484</v>
       </c>
       <c r="F210">
-        <v>-1.183943266104594</v>
+        <v>-6.311287036883249</v>
       </c>
       <c r="G210">
-        <v>-0.02105391660556722</v>
+        <v>-0.07451663651063255</v>
       </c>
       <c r="I210">
         <v>23143.18557343743</v>
@@ -84762,7 +84762,7 @@
         <v>1582.839454628498</v>
       </c>
       <c r="AM210">
-        <v>1601.576484532106</v>
+        <v>1601.576484532107</v>
       </c>
       <c r="AN210">
         <v>5490.301139809075</v>
@@ -84828,7 +84828,7 @@
         <v>-569.7122584012894</v>
       </c>
       <c r="BI210">
-        <v>546.2802971756363</v>
+        <v>546.2802971756362</v>
       </c>
       <c r="BJ210">
         <v>22.09623949328765</v>
@@ -84840,7 +84840,7 @@
         <v>2009.335758674262</v>
       </c>
       <c r="BM210">
-        <v>86.52537346133926</v>
+        <v>86.52537346133927</v>
       </c>
       <c r="BN210">
         <v>0.613723485418602</v>
@@ -84915,7 +84915,7 @@
         <v>23.54858924321161</v>
       </c>
       <c r="CM210">
-        <v>40.71144231210934</v>
+        <v>40.71144231210928</v>
       </c>
       <c r="CN210">
         <v>0</v>
@@ -84957,7 +84957,7 @@
         <v>3.32770703651272</v>
       </c>
       <c r="DA210">
-        <v>0.1454597978205499</v>
+        <v>0.1454597978205356</v>
       </c>
       <c r="DB210">
         <v>0</v>
@@ -84975,10 +84975,10 @@
         <v>8.472431761809116</v>
       </c>
       <c r="DG210">
-        <v>-82.49910709100902</v>
+        <v>-373.1636504425926</v>
       </c>
       <c r="DH210">
-        <v>-78.0232996472914</v>
+        <v>-368.687842998875</v>
       </c>
       <c r="DI210">
         <v>-4.626036123947453</v>
@@ -85008,7 +85008,7 @@
         <v>-3.273491872591132</v>
       </c>
       <c r="DR210">
-        <v>-0.3822010984371332</v>
+        <v>-0.3822010984371337</v>
       </c>
       <c r="DS210">
         <v>-1.383142985272862</v>
@@ -85020,34 +85020,34 @@
         <v>-3.266098487399295</v>
       </c>
       <c r="DV210">
-        <v>-1.206103768409367</v>
+        <v>-4.268792253166789</v>
       </c>
       <c r="DW210">
-        <v>-1.204646659836183</v>
+        <v>-4.267335144593606</v>
       </c>
       <c r="DX210">
         <v>-0.001457108573178914</v>
       </c>
       <c r="DY210">
-        <v>-67.82388576831615</v>
+        <v>-361.5511176046571</v>
       </c>
       <c r="DZ210">
-        <v>0.1966389434520552</v>
+        <v>0.1966389434520547</v>
       </c>
       <c r="EA210">
-        <v>-68.17075339199805</v>
+        <v>-361.8979852283391</v>
       </c>
       <c r="EB210">
-        <v>0.003432556986623427</v>
+        <v>0.003432556986623419</v>
       </c>
       <c r="EC210">
-        <v>-1.189998236011372</v>
+        <v>-6.317342006790027</v>
       </c>
       <c r="ED210">
         <v>0.3651852664783082</v>
       </c>
       <c r="EE210">
-        <v>-1.440115988542643</v>
+        <v>-6.513997039416234</v>
       </c>
       <c r="EF210">
         <v>-0.02414433801489145</v>
@@ -85059,7 +85059,7 @@
         <v>-2.543549169523317e-05</v>
       </c>
       <c r="EI210">
-        <v>-0.0210284811138719</v>
+        <v>-0.07449120101893723</v>
       </c>
     </row>
     <row r="211">
@@ -85067,10 +85067,10 @@
         <v>44742</v>
       </c>
       <c r="B211">
-        <v>-1.939147293292349</v>
+        <v>-1.976178782683645</v>
       </c>
       <c r="C211">
-        <v>-2.207155427861927</v>
+        <v>-3.466509978054704</v>
       </c>
       <c r="D211">
         <v>-0.01235806542162986</v>
@@ -85079,10 +85079,10 @@
         <v>-0.04498415407605297</v>
       </c>
       <c r="F211">
-        <v>-1.881805073794666</v>
+        <v>-1.918836563185962</v>
       </c>
       <c r="G211">
-        <v>-0.05090679324971561</v>
+        <v>-0.08793828264101218</v>
       </c>
       <c r="I211">
         <v>23369.48049237143</v>
@@ -85241,7 +85241,7 @@
         <v>-572.0139731068915</v>
       </c>
       <c r="BI211">
-        <v>551.6218459945027</v>
+        <v>551.6218459945025</v>
       </c>
       <c r="BJ211">
         <v>22.31229733497988</v>
@@ -85253,7 +85253,7 @@
         <v>2028.983117555671</v>
       </c>
       <c r="BM211">
-        <v>87.37142174242121</v>
+        <v>87.37142174242122</v>
       </c>
       <c r="BN211">
         <v>0.6164046564976617</v>
@@ -85421,7 +85421,7 @@
         <v>-4.339212179352049</v>
       </c>
       <c r="DR211">
-        <v>-0.4033272896143132</v>
+        <v>-0.4033272896143136</v>
       </c>
       <c r="DS211">
         <v>-23.42402895181478</v>
@@ -85433,28 +85433,28 @@
         <v>-8.12770428820545</v>
       </c>
       <c r="DV211">
-        <v>-2.945363407816951</v>
+        <v>-5.08792998542584</v>
       </c>
       <c r="DW211">
-        <v>-2.944024936516592</v>
+        <v>-5.086591514125475</v>
       </c>
       <c r="DX211">
         <v>-0.00133847130036227</v>
       </c>
       <c r="DY211">
-        <v>-108.8774100896652</v>
+        <v>-111.0199766672741</v>
       </c>
       <c r="DZ211">
         <v>-1.341235860137977</v>
       </c>
       <c r="EA211">
-        <v>-107.5361742295272</v>
+        <v>-109.6787408071361</v>
       </c>
       <c r="EB211">
         <v>-0.02318152539341653</v>
       </c>
       <c r="EC211">
-        <v>-1.858623548401249</v>
+        <v>-1.895655037792545</v>
       </c>
       <c r="ED211">
         <v>0.425040527988376</v>
@@ -85472,7 +85472,7 @@
         <v>-2.313374355686798e-05</v>
       </c>
       <c r="EI211">
-        <v>-0.05088365950615881</v>
+        <v>-0.08791514889745525</v>
       </c>
     </row>
     <row r="212">
@@ -85480,10 +85480,10 @@
         <v>44834</v>
       </c>
       <c r="B212">
-        <v>-0.5059642727159844</v>
+        <v>-0.5269966399726116</v>
       </c>
       <c r="C212">
-        <v>-1.540285114272208</v>
+        <v>-2.867217634664341</v>
       </c>
       <c r="D212">
         <v>-0.07352568816414681</v>
@@ -85492,10 +85492,10 @@
         <v>-0.0217634055200784</v>
       </c>
       <c r="F212">
-        <v>-0.4106751790317592</v>
+        <v>-0.4317075462883864</v>
       </c>
       <c r="G212">
-        <v>-0.06574532584487809</v>
+        <v>-0.0867776931015035</v>
       </c>
       <c r="I212">
         <v>23606.09985360315</v>
@@ -85582,7 +85582,7 @@
         <v>1606.23733773305</v>
       </c>
       <c r="AK212">
-        <v>2359.857878414072</v>
+        <v>2359.857878414071</v>
       </c>
       <c r="AL212">
         <v>1629.829296473901</v>
@@ -85591,7 +85591,7 @@
         <v>1637.916013941236</v>
       </c>
       <c r="AN212">
-        <v>5627.603188829208</v>
+        <v>5627.603188829209</v>
       </c>
       <c r="AO212">
         <v>505.882034906478</v>
@@ -85654,19 +85654,19 @@
         <v>-573.9088027254136</v>
       </c>
       <c r="BI212">
-        <v>557.2070967613433</v>
+        <v>557.2070967613431</v>
       </c>
       <c r="BJ212">
-        <v>22.53821256423535</v>
+        <v>22.53821256423534</v>
       </c>
       <c r="BK212">
-        <v>1469.781554993427</v>
+        <v>1469.781554993428</v>
       </c>
       <c r="BL212">
         <v>2049.526864319006</v>
       </c>
       <c r="BM212">
-        <v>88.25606999163443</v>
+        <v>88.25606999163445</v>
       </c>
       <c r="BN212">
         <v>0.619120081794921</v>
@@ -85738,7 +85738,7 @@
         <v>-53.35523078998699</v>
       </c>
       <c r="CL212">
-        <v>19.36460641326175</v>
+        <v>19.36460641326266</v>
       </c>
       <c r="CM212">
         <v>39.70032229713371</v>
@@ -85780,7 +85780,7 @@
         <v>3.616944075548076</v>
       </c>
       <c r="CZ212">
-        <v>2.389457637956184</v>
+        <v>2.389457637956639</v>
       </c>
       <c r="DA212">
         <v>0.1028940601896267</v>
@@ -85834,40 +85834,40 @@
         <v>-6.472719702070849</v>
       </c>
       <c r="DR212">
-        <v>-0.3885554389958041</v>
+        <v>-0.3885554389958046</v>
       </c>
       <c r="DS212">
-        <v>-14.91838297386854</v>
+        <v>-14.91838297386865</v>
       </c>
       <c r="DT212">
         <v>-8.792792015219611</v>
       </c>
       <c r="DU212">
-        <v>-6.125590958648955</v>
+        <v>-6.125590958649009</v>
       </c>
       <c r="DV212">
-        <v>-3.841085274491204</v>
+        <v>-5.069874015271451</v>
       </c>
       <c r="DW212">
-        <v>-3.839821882933919</v>
+        <v>-5.06861062371416</v>
       </c>
       <c r="DX212">
         <v>-0.001263391557282836</v>
       </c>
       <c r="DY212">
-        <v>-23.9931639627096</v>
+        <v>-25.22195270348995</v>
       </c>
       <c r="DZ212">
-        <v>1.342251222857678</v>
+        <v>1.342251222857623</v>
       </c>
       <c r="EA212">
-        <v>-25.33541518556731</v>
+        <v>-26.56420392634755</v>
       </c>
       <c r="EB212">
-        <v>0.0229744298046477</v>
+        <v>0.02297442980464676</v>
       </c>
       <c r="EC212">
-        <v>-0.4336496088364075</v>
+        <v>-0.4546819760930327</v>
       </c>
       <c r="ED212">
         <v>0.4964854674221581</v>
@@ -85876,7 +85876,7 @@
         <v>-0.468627262747936</v>
       </c>
       <c r="EF212">
-        <v>-0.255348132000425</v>
+        <v>-0.2553481320004268</v>
       </c>
       <c r="EG212">
         <v>-0.1174399258606781</v>
@@ -85885,7 +85885,7 @@
         <v>-2.162464086773771e-05</v>
       </c>
       <c r="EI212">
-        <v>-0.06572370120401032</v>
+        <v>-0.08675606846063562</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mpc ppp round 2
</commit_message>
<xml_diff>
--- a/results/12-2020/fim.xlsx
+++ b/results/12-2020/fim.xlsx
@@ -83619,22 +83619,22 @@
         <v>44286</v>
       </c>
       <c r="B206">
-        <v>6.807648377777404</v>
+        <v>4.378374994833019</v>
       </c>
       <c r="C206">
-        <v>5.369168832839658</v>
+        <v>4.761850487103561</v>
       </c>
       <c r="D206">
-        <v>0.1642490337702944</v>
+        <v>0.1642490337702973</v>
       </c>
       <c r="E206">
-        <v>3.100508840408109</v>
+        <v>0.974451668876546</v>
       </c>
       <c r="F206">
-        <v>3.542890503599001</v>
+        <v>3.239674292186175</v>
       </c>
       <c r="G206">
-        <v>0.2531305103579604</v>
+        <v>0.3118334335866014</v>
       </c>
       <c r="I206">
         <v>21942.91648059992</v>
@@ -83667,7 +83667,7 @@
         <v>523.17084771922</v>
       </c>
       <c r="S206">
-        <v>472.8009954476429</v>
+        <v>358.0739954476429</v>
       </c>
       <c r="T206">
         <v>74.70668003712791</v>
@@ -83676,7 +83676,7 @@
         <v>0.003938982612060604</v>
       </c>
       <c r="V206">
-        <v>2532.023060624999</v>
+        <v>2417.296060624999</v>
       </c>
       <c r="W206">
         <v>0.0031885362715387</v>
@@ -83718,7 +83718,7 @@
         <v>3703.464861448391</v>
       </c>
       <c r="AJ206">
-        <v>3238.368889579091</v>
+        <v>3151.568889579091</v>
       </c>
       <c r="AK206">
         <v>2219.828214992802</v>
@@ -83736,7 +83736,7 @@
         <v>307.6031794471426</v>
       </c>
       <c r="AP206">
-        <v>500.8542546295093</v>
+        <v>555.5202546295093</v>
       </c>
       <c r="AQ206">
         <v>0</v>
@@ -83754,7 +83754,7 @@
         <v>0</v>
       </c>
       <c r="AV206">
-        <v>3776.984346204091</v>
+        <v>3690.184346204091</v>
       </c>
       <c r="AW206">
         <v>1701.879512646469</v>
@@ -83772,7 +83772,7 @@
         <v>225.5633104395484</v>
       </c>
       <c r="BB206">
-        <v>500.2502499999998</v>
+        <v>554.9162499999998</v>
       </c>
       <c r="BC206">
         <v>220.8917747488439</v>
@@ -83826,16 +83826,16 @@
         <v>53.36225624681128</v>
       </c>
       <c r="BT206">
-        <v>1723.726753352801</v>
+        <v>1636.926753352801</v>
       </c>
       <c r="BU206">
-        <v>-720.5437736769309</v>
+        <v>-665.8777736769309</v>
       </c>
       <c r="BV206">
-        <v>259.2746476487297</v>
+        <v>144.5476476487297</v>
       </c>
       <c r="BW206">
-        <v>190.66</v>
+        <v>75.93300000000001</v>
       </c>
       <c r="BY206">
         <v>244</v>
@@ -83850,10 +83850,10 @@
         <v>-0.09199623047137026</v>
       </c>
       <c r="CC206">
-        <v>3.356754104649774</v>
+        <v>1.230696933118214</v>
       </c>
       <c r="CD206">
-        <v>3.196039472394279</v>
+        <v>1.069982300862716</v>
       </c>
       <c r="CE206">
         <v>-0.003534401514799262</v>
@@ -83862,22 +83862,22 @@
         <v>-0.09199623047137026</v>
       </c>
       <c r="CG206">
-        <v>3.19250507087948</v>
+        <v>1.066447899347916</v>
       </c>
       <c r="CH206">
-        <v>3.356754104649774</v>
+        <v>1.230696933118214</v>
       </c>
       <c r="CI206">
-        <v>3.264757874178404</v>
+        <v>1.138700702646843</v>
       </c>
       <c r="CJ206">
-        <v>115.1875626010849</v>
+        <v>169.8535626010848</v>
       </c>
       <c r="CK206">
         <v>13.02143192736162</v>
       </c>
       <c r="CL206">
-        <v>1208.124904496274</v>
+        <v>1121.324904496274</v>
       </c>
       <c r="CM206">
         <v>31.62146729067354</v>
@@ -83892,13 +83892,13 @@
         <v>-95.67840566666672</v>
       </c>
       <c r="CQ206">
-        <v>115.1888702667205</v>
+        <v>169.8548702667204</v>
       </c>
       <c r="CR206">
         <v>12.19845212836162</v>
       </c>
       <c r="CS206">
-        <v>1206.297289068417</v>
+        <v>1119.497289068417</v>
       </c>
       <c r="CT206">
         <v>10.96059380563247</v>
@@ -83943,10 +83943,10 @@
         <v>-3.748618644962366</v>
       </c>
       <c r="DH206">
-        <v>149.3016789922159</v>
+        <v>129.7716789922158</v>
       </c>
       <c r="DI206">
-        <v>331.3973135441231</v>
+        <v>311.867313544123</v>
       </c>
       <c r="DJ206">
         <v>-182.7973550515025</v>
@@ -83988,34 +83988,34 @@
         <v>-2.900958275664812</v>
       </c>
       <c r="DW206">
-        <v>13.65951228908737</v>
+        <v>16.82725884051275</v>
       </c>
       <c r="DX206">
-        <v>13.66135664064446</v>
+        <v>16.82930310429972</v>
       </c>
       <c r="DY206">
-        <v>-0.001844351557086037</v>
+        <v>-0.002044263786970295</v>
       </c>
       <c r="DZ206">
-        <v>191.1826286936556</v>
+        <v>174.820375245081</v>
       </c>
       <c r="EA206">
-        <v>-190.1384853775714</v>
+        <v>-190.1386852898013</v>
       </c>
       <c r="EB206">
-        <v>380.6193935716317</v>
+        <v>364.2573400352869</v>
       </c>
       <c r="EC206">
-        <v>-3.523541018427528</v>
+        <v>-3.523544723090162</v>
       </c>
       <c r="ED206">
-        <v>7.053427626687371</v>
+        <v>6.750215119937179</v>
       </c>
       <c r="EE206">
         <v>0.4887933070952966</v>
       </c>
       <c r="EF206">
-        <v>2.766775958084007</v>
+        <v>2.404856823442541</v>
       </c>
       <c r="EG206">
         <v>0.05809582119573258</v>
@@ -84024,10 +84024,10 @@
         <v>-0.0239050931339964</v>
       </c>
       <c r="EI206">
-        <v>-3.417850074322673e-05</v>
+        <v>-3.788316337732589e-05</v>
       </c>
       <c r="EJ206">
-        <v>0.2531646888587037</v>
+        <v>0.3118713167499788</v>
       </c>
     </row>
     <row r="207">
@@ -84035,22 +84035,22 @@
         <v>44377</v>
       </c>
       <c r="B207">
-        <v>-3.020017250891981</v>
+        <v>-2.797863445655844</v>
       </c>
       <c r="C207">
-        <v>1.041720123925258</v>
+        <v>0.4899402294981954</v>
       </c>
       <c r="D207">
         <v>0.2541332789429298</v>
       </c>
       <c r="E207">
-        <v>-0.7037459759121391</v>
+        <v>-0.6840515148295346</v>
       </c>
       <c r="F207">
-        <v>-2.570404553922772</v>
+        <v>-2.36794520976924</v>
       </c>
       <c r="G207">
-        <v>0.2208540867683731</v>
+        <v>0.2075232220605232</v>
       </c>
       <c r="I207">
         <v>22291.8404896825</v>
@@ -84083,7 +84083,7 @@
         <v>541.72027157883</v>
       </c>
       <c r="S207">
-        <v>445.6824339220724</v>
+        <v>330.9554339220724</v>
       </c>
       <c r="T207">
         <v>75.04939368825832</v>
@@ -84092,7 +84092,7 @@
         <v>0.00541033706720695</v>
       </c>
       <c r="V207">
-        <v>2537.876468276562</v>
+        <v>2423.149468276562</v>
       </c>
       <c r="W207">
         <v>0.005802914123625325</v>
@@ -84134,7 +84134,7 @@
         <v>3480.13672405082</v>
       </c>
       <c r="AJ207">
-        <v>1801.752352523123</v>
+        <v>1853.752352523123</v>
       </c>
       <c r="AK207">
         <v>2235.404102455741</v>
@@ -84152,7 +84152,7 @@
         <v>319.0393868682636</v>
       </c>
       <c r="AP207">
-        <v>500.8564375574148</v>
+        <v>555.5224375574147</v>
       </c>
       <c r="AQ207">
         <v>0</v>
@@ -84170,7 +84170,7 @@
         <v>0</v>
       </c>
       <c r="AV207">
-        <v>2357.864347789686</v>
+        <v>2409.864347789686</v>
       </c>
       <c r="AW207">
         <v>1709.219268969704</v>
@@ -84188,7 +84188,7 @@
         <v>235.6949656593226</v>
       </c>
       <c r="BB207">
-        <v>500.2502500000001</v>
+        <v>554.91625</v>
       </c>
       <c r="BC207">
         <v>228.723662123266</v>
@@ -84242,16 +84242,16 @@
         <v>63.46748462381947</v>
       </c>
       <c r="BT207">
-        <v>517.2278108710334</v>
+        <v>569.2278108710334</v>
       </c>
       <c r="BU207">
-        <v>-724.95583479476</v>
+        <v>-670.2898347947601</v>
       </c>
       <c r="BV207">
-        <v>247.3259435835118</v>
+        <v>132.5989435835118</v>
       </c>
       <c r="BW207">
-        <v>190.66</v>
+        <v>75.93300000000001</v>
       </c>
       <c r="BY207">
         <v>152</v>
@@ -84266,10 +84266,10 @@
         <v>-0.1216587100175547</v>
       </c>
       <c r="CC207">
-        <v>-0.3279539869516546</v>
+        <v>-0.3082595258690501</v>
       </c>
       <c r="CD207">
-        <v>-0.5755102083040079</v>
+        <v>-0.5558157472214035</v>
       </c>
       <c r="CE207">
         <v>-0.006577057590576529</v>
@@ -84278,22 +84278,22 @@
         <v>-0.1216587100175547</v>
       </c>
       <c r="CG207">
-        <v>-0.5820872658945844</v>
+        <v>-0.56239280481198</v>
       </c>
       <c r="CH207">
-        <v>-0.3279539869516546</v>
+        <v>-0.3082595258690501</v>
       </c>
       <c r="CI207">
-        <v>-0.4496126969692092</v>
+        <v>-0.4299182358866048</v>
       </c>
       <c r="CJ207">
-        <v>-3.528322195847522</v>
+        <v>-3.913661027076614</v>
       </c>
       <c r="CK207">
         <v>4.714920809861496</v>
       </c>
       <c r="CL207">
-        <v>-1365.72374461056</v>
+        <v>-1226.311894273043</v>
       </c>
       <c r="CM207">
         <v>22.71474157470857</v>
@@ -84308,13 +84308,13 @@
         <v>-93.71994795338804</v>
       </c>
       <c r="CQ207">
-        <v>-3.526247515038108</v>
+        <v>-3.9115863462672</v>
       </c>
       <c r="CR207">
         <v>6.041035998057851</v>
       </c>
       <c r="CS207">
-        <v>-1368.446826581655</v>
+        <v>-1229.034976244138</v>
       </c>
       <c r="CT207">
         <v>5.848839984691949</v>
@@ -84359,10 +84359,10 @@
         <v>5.993578954459299</v>
       </c>
       <c r="DH207">
-        <v>-168.8239233496935</v>
+        <v>-156.9862570237522</v>
       </c>
       <c r="DI207">
-        <v>9.361188756162846</v>
+        <v>21.19885508210415</v>
       </c>
       <c r="DJ207">
         <v>-173.1076892043021</v>
@@ -84404,34 +84404,34 @@
         <v>-1.103668719509892</v>
       </c>
       <c r="DW207">
-        <v>12.11545695089395</v>
+        <v>11.38416182364763</v>
       </c>
       <c r="DX207">
-        <v>12.11715741914491</v>
+        <v>11.38604528837508</v>
       </c>
       <c r="DY207">
-        <v>-0.001700468250960165</v>
+        <v>-0.001883464727441673</v>
       </c>
       <c r="DZ207">
-        <v>-141.0054311202027</v>
+        <v>-129.8990599215077</v>
       </c>
       <c r="EA207">
-        <v>-168.7719228513818</v>
+        <v>-168.7721058478583</v>
       </c>
       <c r="EB207">
-        <v>32.84391463273327</v>
+        <v>43.95046882790474</v>
       </c>
       <c r="EC207">
-        <v>-3.076563190687906</v>
+        <v>-3.076566526552154</v>
       </c>
       <c r="ED207">
-        <v>0.5987155747827977</v>
+        <v>0.8011782548005782</v>
       </c>
       <c r="EE207">
         <v>0.2405705283812016</v>
       </c>
       <c r="EF207">
-        <v>-3.077511113875011</v>
+        <v>-2.861720905013628</v>
       </c>
       <c r="EG207">
         <v>0.06331313466601252</v>
@@ -84440,10 +84440,10 @@
         <v>-0.01763118986334844</v>
       </c>
       <c r="EI207">
-        <v>-3.099803533342663e-05</v>
+        <v>-3.433389958179668e-05</v>
       </c>
       <c r="EJ207">
-        <v>0.2208850848037065</v>
+        <v>0.2075575559601051</v>
       </c>
     </row>
     <row r="208">
@@ -84451,22 +84451,22 @@
         <v>44469</v>
       </c>
       <c r="B208">
-        <v>-2.956577902985297</v>
+        <v>-2.912034116707706</v>
       </c>
       <c r="C208">
-        <v>-0.6191846308248271</v>
+        <v>-1.159828578682492</v>
       </c>
       <c r="D208">
-        <v>-0.1580530711298772</v>
+        <v>-0.1580530711298803</v>
       </c>
       <c r="E208">
-        <v>-0.1499749553841785</v>
+        <v>-0.1304715522525736</v>
       </c>
       <c r="F208">
-        <v>-2.648549876471242</v>
+        <v>-2.623509493325252</v>
       </c>
       <c r="G208">
-        <v>0.2383302966107768</v>
+        <v>0.2625192221942464</v>
       </c>
       <c r="I208">
         <v>22664.78462982512</v>
@@ -84499,7 +84499,7 @@
         <v>560.2696954384398</v>
       </c>
       <c r="S208">
-        <v>446.7149761349775</v>
+        <v>331.9879761349775</v>
       </c>
       <c r="T208">
         <v>75.45085825101107</v>
@@ -84508,7 +84508,7 @@
         <v>0.004676012656119388</v>
       </c>
       <c r="V208">
-        <v>2549.612550617944</v>
+        <v>2434.885550617944</v>
       </c>
       <c r="W208">
         <v>0.005585189534516033</v>
@@ -84568,7 +84568,7 @@
         <v>330.5654004191876</v>
       </c>
       <c r="AP208">
-        <v>500.8587948704311</v>
+        <v>555.524794870431</v>
       </c>
       <c r="AQ208">
         <v>0</v>
@@ -84604,7 +84604,7 @@
         <v>245.8266208790969</v>
       </c>
       <c r="BB208">
-        <v>500.2502500000003</v>
+        <v>554.9162500000002</v>
       </c>
       <c r="BC208">
         <v>236.5555494976879</v>
@@ -84661,13 +84661,13 @@
         <v>495.3425409759989</v>
       </c>
       <c r="BU208">
-        <v>-729.7203572857679</v>
+        <v>-675.054357285768</v>
       </c>
       <c r="BV208">
-        <v>262.9489890168967</v>
+        <v>148.2219890168967</v>
       </c>
       <c r="BW208">
-        <v>190.66</v>
+        <v>75.93300000000001</v>
       </c>
       <c r="BY208">
         <v>44</v>
@@ -84682,10 +84682,10 @@
         <v>-0.0871829025843979</v>
       </c>
       <c r="CC208">
-        <v>-0.2208451239296579</v>
+        <v>-0.201341720798056</v>
       </c>
       <c r="CD208">
-        <v>-0.05723757203912079</v>
+        <v>-0.03773416890751585</v>
       </c>
       <c r="CE208">
         <v>-0.005554480760659826</v>
@@ -84694,22 +84694,22 @@
         <v>-0.0871829025843979</v>
       </c>
       <c r="CG208">
-        <v>-0.06279205279978062</v>
+        <v>-0.04328864966817567</v>
       </c>
       <c r="CH208">
-        <v>-0.2208451239296579</v>
+        <v>-0.201341720798056</v>
       </c>
       <c r="CI208">
-        <v>-0.3080280265140558</v>
+        <v>-0.2885246233824539</v>
       </c>
       <c r="CJ208">
-        <v>-3.859585526331614</v>
+        <v>-4.281097463535389</v>
       </c>
       <c r="CK208">
         <v>-1.614949901188083</v>
       </c>
       <c r="CL208">
-        <v>-78.00748108314201</v>
+        <v>-130.408436352132</v>
       </c>
       <c r="CM208">
         <v>20.87980333247287</v>
@@ -84724,13 +84724,13 @@
         <v>-109.1720230939701</v>
       </c>
       <c r="CQ208">
-        <v>-3.857268722133426</v>
+        <v>-4.278780659337144</v>
       </c>
       <c r="CR208">
         <v>-0.1643476347387605</v>
       </c>
       <c r="CS208">
-        <v>-79.6341916161573</v>
+        <v>-132.0351468851472</v>
       </c>
       <c r="CT208">
         <v>3.422631669898237</v>
@@ -84775,10 +84775,10 @@
         <v>-4.933260291017048</v>
       </c>
       <c r="DH208">
-        <v>-168.0597944897011</v>
+        <v>-168.0123430992825</v>
       </c>
       <c r="DI208">
-        <v>-26.65409639042004</v>
+        <v>-26.60664500000147</v>
       </c>
       <c r="DJ208">
         <v>-140.8212576788797</v>
@@ -84820,34 +84820,34 @@
         <v>-4.157792792855044</v>
       </c>
       <c r="DW208">
-        <v>13.28205238976538</v>
+        <v>14.63009156657415</v>
       </c>
       <c r="DX208">
-        <v>13.28364900368908</v>
+        <v>14.631853661348</v>
       </c>
       <c r="DY208">
-        <v>-0.001596613923682332</v>
+        <v>-0.001762094773837164</v>
       </c>
       <c r="DZ208">
-        <v>-147.6026284381631</v>
+        <v>-146.2071378709357</v>
       </c>
       <c r="EA208">
-        <v>-150.4652442672989</v>
+        <v>-150.465409748149</v>
       </c>
       <c r="EB208">
-        <v>3.447056249537128</v>
+        <v>4.842712297614612</v>
       </c>
       <c r="EC208">
-        <v>-2.69991604034561</v>
+        <v>-2.699919009698459</v>
       </c>
       <c r="ED208">
-        <v>0.06185323730685323</v>
+        <v>0.08689658980569145</v>
       </c>
       <c r="EE208">
         <v>0.1398026042248747</v>
       </c>
       <c r="EF208">
-        <v>-3.015628872232159</v>
+        <v>-3.014777414669639</v>
       </c>
       <c r="EG208">
         <v>0.006609512793869101</v>
@@ -84856,10 +84856,10 @@
         <v>-0.01766341786860341</v>
       </c>
       <c r="EI208">
-        <v>-2.864929747584198e-05</v>
+        <v>-3.161865032459258e-05</v>
       </c>
       <c r="EJ208">
-        <v>0.2383589459082528</v>
+        <v>0.2625508408445711</v>
       </c>
     </row>
     <row r="209">
@@ -84867,22 +84867,22 @@
         <v>44561</v>
       </c>
       <c r="B209">
-        <v>-5.994976992591383</v>
+        <v>-2.820587636041925</v>
       </c>
       <c r="C209">
-        <v>-1.290980942172814</v>
+        <v>-1.038027550893114</v>
       </c>
       <c r="D209">
-        <v>0.03569302105791428</v>
+        <v>0.03569302105791516</v>
       </c>
       <c r="E209">
-        <v>-3.554553272110574</v>
+        <v>-0.1701103953747071</v>
       </c>
       <c r="F209">
-        <v>-2.476116741538723</v>
+        <v>-2.686170261725133</v>
       </c>
       <c r="G209">
-        <v>-0.1016616536958829</v>
+        <v>-0.3125526208943607</v>
       </c>
       <c r="I209">
         <v>22914.57292255905</v>
@@ -84915,7 +84915,7 @@
         <v>554.6929574085671</v>
       </c>
       <c r="S209">
-        <v>251.544379693251</v>
+        <v>327.477379693251</v>
       </c>
       <c r="T209">
         <v>76.02995588093096</v>
@@ -84924,7 +84924,7 @@
         <v>0.004663517061526345</v>
       </c>
       <c r="V209">
-        <v>2376.644694747579</v>
+        <v>2452.577694747579</v>
       </c>
       <c r="W209">
         <v>0.005492326385298174</v>
@@ -85080,10 +85080,10 @@
         <v>-1134.856223009233</v>
       </c>
       <c r="BV209">
-        <v>56.49105945954122</v>
+        <v>132.4240594595412</v>
       </c>
       <c r="BW209">
-        <v>0</v>
+        <v>75.93300000000001</v>
       </c>
       <c r="BY209">
         <v>44</v>
@@ -85098,10 +85098,10 @@
         <v>-0.03120613930242417</v>
       </c>
       <c r="CC209">
-        <v>-3.487654111750235</v>
+        <v>-0.1032112350143678</v>
       </c>
       <c r="CD209">
-        <v>-3.520693575869183</v>
+        <v>-0.136250699133316</v>
       </c>
       <c r="CE209">
         <v>-0.002653556938966896</v>
@@ -85110,16 +85110,16 @@
         <v>-0.03120613930242417</v>
       </c>
       <c r="CG209">
-        <v>-3.52334713280815</v>
+        <v>-0.1389042560722829</v>
       </c>
       <c r="CH209">
-        <v>-3.487654111750235</v>
+        <v>-0.1032112350143678</v>
       </c>
       <c r="CI209">
-        <v>-3.51886025105266</v>
+        <v>-0.1344173743167919</v>
       </c>
       <c r="CJ209">
-        <v>-403.802998777228</v>
+        <v>-458.8843526489966</v>
       </c>
       <c r="CK209">
         <v>23.90952447025347</v>
@@ -85140,7 +85140,7 @@
         <v>-0.3343132908538493</v>
       </c>
       <c r="CQ209">
-        <v>-403.8009160756357</v>
+        <v>-458.8822699474042</v>
       </c>
       <c r="CR209">
         <v>25.33893420835716</v>
@@ -85191,10 +85191,10 @@
         <v>-0.7612081635936206</v>
       </c>
       <c r="DH209">
-        <v>-140.1961841027644</v>
+        <v>-140.1487327123459</v>
       </c>
       <c r="DI209">
-        <v>-130.2630874448699</v>
+        <v>-130.2156360544513</v>
       </c>
       <c r="DJ209">
         <v>-11.20657095841259</v>
@@ -85236,34 +85236,34 @@
         <v>-4.864471821940306</v>
       </c>
       <c r="DW209">
-        <v>-5.760348715322626</v>
+        <v>-17.70984459514516</v>
       </c>
       <c r="DX209">
-        <v>-5.758851557342008</v>
+        <v>-17.70818701438939</v>
       </c>
       <c r="DY209">
-        <v>-0.001497157980611642</v>
+        <v>-0.001657580755759397</v>
       </c>
       <c r="DZ209">
-        <v>-140.3016316631988</v>
+        <v>-152.2036761526028</v>
       </c>
       <c r="EA209">
-        <v>-17.36502768106773</v>
+        <v>-17.36518810384288</v>
       </c>
       <c r="EB209">
-        <v>-124.2100782826491</v>
+        <v>-136.1119623492779</v>
       </c>
       <c r="EC209">
-        <v>-0.3064671112421106</v>
+        <v>-0.3064699424673398</v>
       </c>
       <c r="ED209">
-        <v>-2.192124572305851</v>
+        <v>-2.402175261267031</v>
       </c>
       <c r="EE209">
         <v>0.1589595275846998</v>
       </c>
       <c r="EF209">
-        <v>-2.474255747716694</v>
+        <v>-2.473418300704625</v>
       </c>
       <c r="EG209">
         <v>-0.02900072934574374</v>
@@ -85272,10 +85272,10 @@
         <v>-0.03015813836510257</v>
       </c>
       <c r="EI209">
-        <v>-2.642262885024721e-05</v>
+        <v>-2.92538540794806e-05</v>
       </c>
       <c r="EJ209">
-        <v>-0.1016352310670325</v>
+        <v>-0.3125233670402811</v>
       </c>
     </row>
     <row r="210">
@@ -85283,22 +85283,22 @@
         <v>44651</v>
       </c>
       <c r="B210">
-        <v>-6.368117040881671</v>
+        <v>-6.166515983169825</v>
       </c>
       <c r="C210">
-        <v>-4.584922296837583</v>
+        <v>-3.674250295393825</v>
       </c>
       <c r="D210">
-        <v>0.09133680375806208</v>
+        <v>0.09133680375806255</v>
       </c>
       <c r="E210">
-        <v>-0.148166807756484</v>
+        <v>-0.162513297365059</v>
       </c>
       <c r="F210">
-        <v>-6.311287036883249</v>
+        <v>-6.095339489562829</v>
       </c>
       <c r="G210">
-        <v>-0.07451663651063255</v>
+        <v>-0.2003158275052838</v>
       </c>
       <c r="I210">
         <v>23143.18557343743</v>
@@ -85331,7 +85331,7 @@
         <v>549.1162193786943</v>
       </c>
       <c r="S210">
-        <v>247.2408068497152</v>
+        <v>323.1738068497152</v>
       </c>
       <c r="T210">
         <v>76.68954672196401</v>
@@ -85340,7 +85340,7 @@
         <v>0.005207433285125074</v>
       </c>
       <c r="V210">
-        <v>2400.411141695055</v>
+        <v>2476.344141695055</v>
       </c>
       <c r="W210">
         <v>0.006507269187908227</v>
@@ -85496,10 +85496,10 @@
         <v>-1165.607201278565</v>
       </c>
       <c r="BV210">
-        <v>40.1063941892165</v>
+        <v>116.0393941892165</v>
       </c>
       <c r="BW210">
-        <v>0</v>
+        <v>75.93300000000001</v>
       </c>
       <c r="BY210">
         <v>44</v>
@@ -85514,10 +85514,10 @@
         <v>-0.02266630882949239</v>
       </c>
       <c r="CC210">
-        <v>-0.03416369516892951</v>
+        <v>-0.04851018477750409</v>
       </c>
       <c r="CD210">
-        <v>-0.1226496011123299</v>
+        <v>-0.136996090720905</v>
       </c>
       <c r="CE210">
         <v>-0.002850897814661666</v>
@@ -85526,13 +85526,13 @@
         <v>-0.02266630882949239</v>
       </c>
       <c r="CG210">
-        <v>-0.1255004989269916</v>
+        <v>-0.1398469885355667</v>
       </c>
       <c r="CH210">
-        <v>-0.03416369516892951</v>
+        <v>-0.04851018477750409</v>
       </c>
       <c r="CI210">
-        <v>-0.05683000399842189</v>
+        <v>-0.07117649360699649</v>
       </c>
       <c r="CJ210">
         <v>-26.24997409540397</v>
@@ -85607,10 +85607,10 @@
         <v>8.472431761809116</v>
       </c>
       <c r="DH210">
-        <v>-373.1636504425926</v>
+        <v>-353.586199052174</v>
       </c>
       <c r="DI210">
-        <v>-368.687842998875</v>
+        <v>-349.1103916084563</v>
       </c>
       <c r="DJ210">
         <v>-4.626036123947453</v>
@@ -85652,34 +85652,34 @@
         <v>-3.266098487399295</v>
       </c>
       <c r="DW210">
-        <v>-4.268792253166789</v>
+        <v>-11.47537909228146</v>
       </c>
       <c r="DX210">
-        <v>-4.267335144593606</v>
+        <v>-11.47375929295095</v>
       </c>
       <c r="DY210">
-        <v>-0.001457108573178914</v>
+        <v>-0.001619799330510879</v>
       </c>
       <c r="DZ210">
-        <v>-361.5511176046571</v>
+        <v>-349.1802530533532</v>
       </c>
       <c r="EA210">
-        <v>0.1966389434520547</v>
+        <v>0.1964762526947227</v>
       </c>
       <c r="EB210">
-        <v>-361.8979852283391</v>
+        <v>-349.5269579862778</v>
       </c>
       <c r="EC210">
-        <v>0.003432556986623419</v>
+        <v>0.003429717033936859</v>
       </c>
       <c r="ED210">
-        <v>-6.317342006790027</v>
+        <v>-6.101391619516919</v>
       </c>
       <c r="EE210">
         <v>0.3651852664783082</v>
       </c>
       <c r="EF210">
-        <v>-6.513997039416234</v>
+        <v>-6.172250301101161</v>
       </c>
       <c r="EG210">
         <v>-0.02414433801489145</v>
@@ -85688,10 +85688,10 @@
         <v>-0.06381428941980051</v>
       </c>
       <c r="EI210">
-        <v>-2.543549169523317e-05</v>
+        <v>-2.827544438179271e-05</v>
       </c>
       <c r="EJ210">
-        <v>-0.07449120101893723</v>
+        <v>-0.2002875520609019</v>
       </c>
     </row>
     <row r="211">
@@ -85699,22 +85699,22 @@
         <v>44742</v>
       </c>
       <c r="B211">
-        <v>-1.976178782683645</v>
+        <v>-2.352309585936044</v>
       </c>
       <c r="C211">
-        <v>-4.323962679785499</v>
+        <v>-3.562861830463875</v>
       </c>
       <c r="D211">
-        <v>-0.01235806542162986</v>
+        <v>-0.01235806542162494</v>
       </c>
       <c r="E211">
-        <v>-0.04498415407605297</v>
+        <v>-0.05990943407882802</v>
       </c>
       <c r="F211">
-        <v>-1.918836563185962</v>
+        <v>-2.280042086435591</v>
       </c>
       <c r="G211">
-        <v>-0.08793828264101218</v>
+        <v>-0.2453652050906725</v>
       </c>
       <c r="I211">
         <v>23369.48049237143</v>
@@ -85747,7 +85747,7 @@
         <v>543.5394813488216</v>
       </c>
       <c r="S211">
-        <v>248.9585717819477</v>
+        <v>324.8915717819477</v>
       </c>
       <c r="T211">
         <v>77.35743394130677</v>
@@ -85756,7 +85756,7 @@
         <v>0.005185091302505995</v>
       </c>
       <c r="V211">
-        <v>2425.696511786188</v>
+        <v>2501.629511786188</v>
       </c>
       <c r="W211">
         <v>0.007003781629901784</v>
@@ -85912,10 +85912,10 @@
         <v>-1170.699384308648</v>
       </c>
       <c r="BV211">
-        <v>29.66125448414999</v>
+        <v>105.59425448415</v>
       </c>
       <c r="BW211">
-        <v>0</v>
+        <v>75.93300000000001</v>
       </c>
       <c r="BY211">
         <v>44</v>
@@ -85930,10 +85930,10 @@
         <v>-0.02254578389738971</v>
       </c>
       <c r="CC211">
-        <v>-0.03479643560029311</v>
+        <v>-0.04972171560306325</v>
       </c>
       <c r="CD211">
-        <v>-0.01890795035009755</v>
+        <v>-0.03383323035287261</v>
       </c>
       <c r="CE211">
         <v>-0.0035304198285657</v>
@@ -85942,13 +85942,13 @@
         <v>-0.02254578389738971</v>
       </c>
       <c r="CG211">
-        <v>-0.02243837017866325</v>
+        <v>-0.03736365018143831</v>
       </c>
       <c r="CH211">
-        <v>-0.03479643560029311</v>
+        <v>-0.04972171560306325</v>
       </c>
       <c r="CI211">
-        <v>-0.05734221949768283</v>
+        <v>-0.07226749950045297</v>
       </c>
       <c r="CJ211">
         <v>-0.3310020145693642</v>
@@ -86023,10 +86023,10 @@
         <v>8.314639657075636</v>
       </c>
       <c r="DH211">
-        <v>-102.3574577997341</v>
+        <v>-114.1476727352568</v>
       </c>
       <c r="DI211">
-        <v>-101.2339523316406</v>
+        <v>-113.0241672671634</v>
       </c>
       <c r="DJ211">
         <v>-1.123505468093488</v>
@@ -86068,34 +86068,34 @@
         <v>-8.12770428820545</v>
       </c>
       <c r="DW211">
-        <v>-5.08792998542584</v>
+        <v>-14.19633118669492</v>
       </c>
       <c r="DX211">
-        <v>-5.086591514125475</v>
+        <v>-14.19480567096256</v>
       </c>
       <c r="DY211">
-        <v>-0.00133847130036227</v>
+        <v>-0.001525515732356135</v>
       </c>
       <c r="DZ211">
-        <v>-111.0199766672741</v>
+        <v>-131.9185928040659</v>
       </c>
       <c r="EA211">
-        <v>-1.341235860137977</v>
+        <v>-1.341422904569971</v>
       </c>
       <c r="EB211">
-        <v>-109.6787408071361</v>
+        <v>-130.5771698994959</v>
       </c>
       <c r="EC211">
-        <v>-0.02318152539341653</v>
+        <v>-0.02318475821426396</v>
       </c>
       <c r="ED211">
-        <v>-1.895655037792545</v>
+        <v>-2.256857328221327</v>
       </c>
       <c r="EE211">
         <v>0.425040527988376</v>
       </c>
       <c r="EF211">
-        <v>-1.769116139607242</v>
+        <v>-1.972894740407211</v>
       </c>
       <c r="EG211">
         <v>-0.4048540141975906</v>
@@ -86104,10 +86104,10 @@
         <v>-0.08196865472849357</v>
       </c>
       <c r="EI211">
-        <v>-2.313374355686798e-05</v>
+        <v>-2.636656440428917e-05</v>
       </c>
       <c r="EJ211">
-        <v>-0.08791514889745525</v>
+        <v>-0.2453388385262681</v>
       </c>
     </row>
     <row r="212">
@@ -86115,22 +86115,22 @@
         <v>44834</v>
       </c>
       <c r="B212">
-        <v>-0.5269966399726116</v>
+        <v>-0.6678887022411846</v>
       </c>
       <c r="C212">
-        <v>-3.716567364032327</v>
+        <v>-3.001825476847245</v>
       </c>
       <c r="D212">
-        <v>-0.07352568816414681</v>
+        <v>-0.07352568816414827</v>
       </c>
       <c r="E212">
-        <v>-0.0217634055200784</v>
+        <v>-0.03688906968240128</v>
       </c>
       <c r="F212">
-        <v>-0.4317075462883864</v>
+        <v>-0.557473944394635</v>
       </c>
       <c r="G212">
-        <v>-0.0867776931015035</v>
+        <v>-0.2125440912077522</v>
       </c>
       <c r="I212">
         <v>23606.09985360315</v>
@@ -86163,7 +86163,7 @@
         <v>537.9627433189488</v>
       </c>
       <c r="S212">
-        <v>250.866801250513</v>
+        <v>326.7998012505129</v>
       </c>
       <c r="T212">
         <v>78.09937601365499</v>
@@ -86172,7 +86172,7 @@
         <v>0.005265472378314096</v>
       </c>
       <c r="V212">
-        <v>2448.483327520491</v>
+        <v>2524.416327520491</v>
       </c>
       <c r="W212">
         <v>0.007232591441219238</v>
@@ -86328,10 +86328,10 @@
         <v>-1175.856624264783</v>
       </c>
       <c r="BV212">
-        <v>18.67630991385104</v>
+        <v>94.60930991385104</v>
       </c>
       <c r="BW212">
-        <v>0</v>
+        <v>75.93300000000001</v>
       </c>
       <c r="BY212">
         <v>44</v>
@@ -86346,10 +86346,10 @@
         <v>-0.002123311404910891</v>
       </c>
       <c r="CC212">
-        <v>-0.09316578227931432</v>
+        <v>-0.1082914464416387</v>
       </c>
       <c r="CD212">
-        <v>-0.01693001987003541</v>
+        <v>-0.03205568403235828</v>
       </c>
       <c r="CE212">
         <v>-0.002710074245132106</v>
@@ -86358,13 +86358,13 @@
         <v>-0.002123311404910891</v>
       </c>
       <c r="CG212">
-        <v>-0.01964009411516751</v>
+        <v>-0.03476575827749039</v>
       </c>
       <c r="CH212">
-        <v>-0.09316578227931432</v>
+        <v>-0.1082914464416387</v>
       </c>
       <c r="CI212">
-        <v>-0.09528909368422522</v>
+        <v>-0.1104147578465496</v>
       </c>
       <c r="CJ212">
         <v>-0.3441800154724035</v>
@@ -86484,28 +86484,28 @@
         <v>-6.125590958649009</v>
       </c>
       <c r="DW212">
-        <v>-5.069874015271451</v>
+        <v>-12.41761248312094</v>
       </c>
       <c r="DX212">
-        <v>-5.06861062371416</v>
+        <v>-12.4161721963187</v>
       </c>
       <c r="DY212">
-        <v>-0.001263391557282836</v>
+        <v>-0.00144028680224977</v>
       </c>
       <c r="DZ212">
-        <v>-25.22195270348995</v>
+        <v>-32.56969117133944</v>
       </c>
       <c r="EA212">
-        <v>1.342251222857623</v>
+        <v>1.342074327612656</v>
       </c>
       <c r="EB212">
-        <v>-26.56420392634755</v>
+        <v>-33.91176549895208</v>
       </c>
       <c r="EC212">
-        <v>0.02297442980464676</v>
+        <v>0.02297140200529068</v>
       </c>
       <c r="ED212">
-        <v>-0.4546819760930327</v>
+        <v>-0.5804453463999254</v>
       </c>
       <c r="EE212">
         <v>0.4964854674221581</v>
@@ -86520,10 +86520,10 @@
         <v>-0.1174399258606781</v>
       </c>
       <c r="EI212">
-        <v>-2.162464086773771e-05</v>
+        <v>-2.465244022381974e-05</v>
       </c>
       <c r="EJ212">
-        <v>-0.08675606846063562</v>
+        <v>-0.2125194387675284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
spreading out ppp over two quarters instead of three
</commit_message>
<xml_diff>
--- a/results/12-2020/fim.xlsx
+++ b/results/12-2020/fim.xlsx
@@ -84853,10 +84853,10 @@
         <v>44286</v>
       </c>
       <c r="B206">
-        <v>7.021074301887467</v>
+        <v>7.337069943294125</v>
       </c>
       <c r="C206">
-        <v>5.468111291003594</v>
+        <v>5.547110201355259</v>
       </c>
       <c r="D206">
         <v>0.1641566356977335</v>
@@ -84865,10 +84865,10 @@
         <v>1.982552178870741</v>
       </c>
       <c r="F206">
-        <v>4.874365487318992</v>
+        <v>5.190361128725651</v>
       </c>
       <c r="G206">
-        <v>0.3446112666511491</v>
+        <v>0.6606069080578083</v>
       </c>
       <c r="I206">
         <v>21956.60675467075</v>
@@ -84970,7 +84970,7 @@
         <v>320.9813082499604</v>
       </c>
       <c r="AP206">
-        <v>578.0209212961762</v>
+        <v>794.6875879628429</v>
       </c>
       <c r="AQ206">
         <v>664</v>
@@ -85006,7 +85006,7 @@
         <v>227.4311020993011</v>
       </c>
       <c r="BB206">
-        <v>577.4169166666667</v>
+        <v>794.0835833333334</v>
       </c>
       <c r="BC206">
         <v>212.711714093908</v>
@@ -85063,7 +85063,7 @@
         <v>1035.307634666419</v>
       </c>
       <c r="BU206">
-        <v>-643.5784418867673</v>
+        <v>-426.9117752201006</v>
       </c>
       <c r="BV206">
         <v>127.66634709591</v>
@@ -85111,7 +85111,7 @@
         <v>2.146708814568474</v>
       </c>
       <c r="CL206">
-        <v>192.3542292677524</v>
+        <v>409.0208959344192</v>
       </c>
       <c r="CM206">
         <v>24.94135191264832</v>
@@ -85132,7 +85132,7 @@
         <v>377.2826694083284</v>
       </c>
       <c r="CS206">
-        <v>192.355536933388</v>
+        <v>409.0222036000548</v>
       </c>
       <c r="CT206">
         <v>24.12737734491157</v>
@@ -85228,28 +85228,28 @@
         <v>-5.087834244464831</v>
       </c>
       <c r="DY206">
-        <v>18.60762924153206</v>
+        <v>35.67012924153207</v>
       </c>
       <c r="DZ206">
-        <v>18.60966808584151</v>
+        <v>35.67216808584151</v>
       </c>
       <c r="EA206">
         <v>-0.002038844309449581</v>
       </c>
       <c r="EB206">
-        <v>263.1962287743999</v>
+        <v>280.2587287743999</v>
       </c>
       <c r="EC206">
         <v>-29.19959197334801</v>
       </c>
       <c r="ED206">
-        <v>292.4295391806045</v>
+        <v>309.4920391806045</v>
       </c>
       <c r="EE206">
         <v>-0.5407732626772654</v>
       </c>
       <c r="EF206">
-        <v>5.415763211699861</v>
+        <v>5.731758853106521</v>
       </c>
       <c r="EG206">
         <v>0.50714746520856</v>
@@ -85267,7 +85267,7 @@
         <v>-3.775917452265713e-05</v>
       </c>
       <c r="EL206">
-        <v>0.3446490258256716</v>
+        <v>0.660644667232331</v>
       </c>
     </row>
     <row r="207">
@@ -85275,10 +85275,10 @@
         <v>44377</v>
       </c>
       <c r="B207">
-        <v>-3.676910995405035</v>
+        <v>-3.445971813557383</v>
       </c>
       <c r="C207">
-        <v>0.9764391459609327</v>
+        <v>1.113172851774511</v>
       </c>
       <c r="D207">
         <v>0.2539920360395043</v>
@@ -85287,10 +85287,10 @@
         <v>-0.6924794352765421</v>
       </c>
       <c r="F207">
-        <v>-3.238423596167997</v>
+        <v>-3.007484414320345</v>
       </c>
       <c r="G207">
-        <v>0.2315082653221971</v>
+        <v>0.462447447169849</v>
       </c>
       <c r="I207">
         <v>22305.74845884954</v>
@@ -85392,7 +85392,7 @@
         <v>332.6844424570025</v>
       </c>
       <c r="AP207">
-        <v>578.0231042240816</v>
+        <v>794.6897708907484</v>
       </c>
       <c r="AQ207">
         <v>0</v>
@@ -85428,7 +85428,7 @@
         <v>237.6466531489517</v>
       </c>
       <c r="BB207">
-        <v>577.4169166666669</v>
+        <v>794.0835833333336</v>
       </c>
       <c r="BC207">
         <v>220.2535711408621</v>
@@ -85485,7 +85485,7 @@
         <v>15.26658746833914</v>
       </c>
       <c r="BU207">
-        <v>-647.9912306472314</v>
+        <v>-431.3245639805647</v>
       </c>
       <c r="BV207">
         <v>115.7178801996623</v>
@@ -85533,7 +85533,7 @@
         <v>-0.4384873992370378</v>
       </c>
       <c r="CL207">
-        <v>-4.072267484384838</v>
+        <v>-5.599543672502591</v>
       </c>
       <c r="CM207">
         <v>16.77480021403017</v>
@@ -85554,7 +85554,7 @@
         <v>-577.1034521239875</v>
       </c>
       <c r="CS207">
-        <v>-4.070192803575424</v>
+        <v>-5.59746899169329</v>
       </c>
       <c r="CT207">
         <v>18.08640474963704</v>
@@ -85650,28 +85650,28 @@
         <v>-3.299335569623718</v>
       </c>
       <c r="DY207">
-        <v>12.70783985533865</v>
+        <v>25.38444185552438</v>
       </c>
       <c r="DZ207">
-        <v>12.70971857802327</v>
+        <v>25.38632057820899</v>
       </c>
       <c r="EA207">
         <v>-0.001878722684611048</v>
       </c>
       <c r="EB207">
-        <v>-177.7619835152685</v>
+        <v>-165.0853815150827</v>
       </c>
       <c r="EC207">
         <v>-9.872615621744803</v>
       </c>
       <c r="ED207">
-        <v>-167.9984706779389</v>
+        <v>-155.3218686777531</v>
       </c>
       <c r="EE207">
         <v>-0.1798568555160671</v>
       </c>
       <c r="EF207">
-        <v>-3.06055434803834</v>
+        <v>-2.829615166190687</v>
       </c>
       <c r="EG207">
         <v>0.3082084226760552</v>
@@ -85689,7 +85689,7 @@
         <v>-3.422610252308488e-05</v>
       </c>
       <c r="EL207">
-        <v>0.2315424914247202</v>
+        <v>0.4624816732723722</v>
       </c>
     </row>
     <row r="208">
@@ -85697,10 +85697,10 @@
         <v>44469</v>
       </c>
       <c r="B208">
-        <v>-5.100253827880115</v>
+        <v>-5.818172229432157</v>
       </c>
       <c r="C208">
-        <v>-1.200434040420372</v>
+        <v>-1.243179934994805</v>
       </c>
       <c r="D208">
         <v>-0.157942597920508</v>
@@ -85709,10 +85709,10 @@
         <v>-0.870145153811781</v>
       </c>
       <c r="F208">
-        <v>-4.072166076147826</v>
+        <v>-4.790084477699868</v>
       </c>
       <c r="G208">
-        <v>0.2832336887216613</v>
+        <v>-0.4346847128303811</v>
       </c>
       <c r="I208">
         <v>22678.92528034497</v>
@@ -85814,7 +85814,7 @@
         <v>344.4899827509665</v>
       </c>
       <c r="AP208">
-        <v>578.0254615370975</v>
+        <v>144.6921282037641</v>
       </c>
       <c r="AQ208">
         <v>0</v>
@@ -85850,7 +85850,7 @@
         <v>247.8622041986023</v>
       </c>
       <c r="BB208">
-        <v>577.4169166666667</v>
+        <v>144.0835833333333</v>
       </c>
       <c r="BC208">
         <v>227.795428187816</v>
@@ -85907,7 +85907,7 @@
         <v>-24.53922848281059</v>
       </c>
       <c r="BU208">
-        <v>-652.7565389092453</v>
+        <v>-1086.089872242579</v>
       </c>
       <c r="BV208">
         <v>131.3412034595532</v>
@@ -85955,7 +85955,7 @@
         <v>-1.028087751732289</v>
       </c>
       <c r="CL208">
-        <v>-4.454592864608571</v>
+        <v>-656.1252398187328</v>
       </c>
       <c r="CM208">
         <v>10.55561585641681</v>
@@ -85976,7 +85976,7 @@
         <v>-109.1720230939701</v>
       </c>
       <c r="CS208">
-        <v>-4.452276060410441</v>
+        <v>-656.1229230145345</v>
       </c>
       <c r="CT208">
         <v>11.99034530448557</v>
@@ -86072,28 +86072,28 @@
         <v>-6.369455707423422</v>
       </c>
       <c r="DY208">
-        <v>15.79434853924366</v>
+        <v>-24.23991965825432</v>
       </c>
       <c r="DZ208">
-        <v>15.79610656940936</v>
+        <v>-24.23816162808862</v>
       </c>
       <c r="EA208">
         <v>-0.001758030165696628</v>
       </c>
       <c r="EB208">
-        <v>-227.0817804430343</v>
+        <v>-267.1160486405323</v>
       </c>
       <c r="EC208">
         <v>19.83522232622621</v>
       </c>
       <c r="ED208">
-        <v>-246.9444921482729</v>
+        <v>-286.9787603457709</v>
       </c>
       <c r="EE208">
         <v>0.3556970502526549</v>
       </c>
       <c r="EF208">
-        <v>-4.428356082358683</v>
+        <v>-5.146274483910725</v>
       </c>
       <c r="EG208">
         <v>0.285176891163129</v>
@@ -86111,7 +86111,7 @@
         <v>-3.152604664111418e-05</v>
       </c>
       <c r="EL208">
-        <v>0.2832652147683025</v>
+        <v>-0.43465318678374</v>
       </c>
     </row>
     <row r="209">
@@ -86119,10 +86119,10 @@
         <v>44561</v>
       </c>
       <c r="B209">
-        <v>-2.125316376018882</v>
+        <v>-2.023584427185488</v>
       </c>
       <c r="C209">
-        <v>-0.9703517243541402</v>
+        <v>-0.9876646317202245</v>
       </c>
       <c r="D209">
         <v>0.03567647282246397</v>
@@ -86131,10 +86131,10 @@
         <v>-0.171893517168879</v>
       </c>
       <c r="F209">
-        <v>-1.989099331672467</v>
+        <v>-1.887367382839073</v>
       </c>
       <c r="G209">
-        <v>-0.2945640177754174</v>
+        <v>-0.1928320689420237</v>
       </c>
       <c r="I209">
         <v>22928.86941700194</v>
@@ -86377,7 +86377,7 @@
         <v>-0.136217044346415</v>
       </c>
       <c r="CL209">
-        <v>-459.0559800411114</v>
+        <v>-22.43016732815676</v>
       </c>
       <c r="CM209">
         <v>24.47082542566432</v>
@@ -86398,7 +86398,7 @@
         <v>-0.3343132908538493</v>
       </c>
       <c r="CS209">
-        <v>-459.053897339519</v>
+        <v>-22.42808462656441</v>
       </c>
       <c r="CT209">
         <v>25.88459423883023</v>
@@ -86494,28 +86494,28 @@
         <v>-7.072325958271414</v>
       </c>
       <c r="DY209">
-        <v>-16.70098837351725</v>
+        <v>-10.93306020797622</v>
       </c>
       <c r="DZ209">
-        <v>-16.69933485736962</v>
+        <v>-10.93140669182859</v>
       </c>
       <c r="EA209">
         <v>-0.001653516147618861</v>
       </c>
       <c r="EB209">
-        <v>-112.77658779546</v>
+        <v>-107.008659629919</v>
       </c>
       <c r="EC209">
         <v>-20.80863697487639</v>
       </c>
       <c r="ED209">
-        <v>-91.94058322577864</v>
+        <v>-86.1726550602376</v>
       </c>
       <c r="EE209">
         <v>-0.3670127524589625</v>
       </c>
       <c r="EF209">
-        <v>-1.621603882710621</v>
+        <v>-1.519871933877226</v>
       </c>
       <c r="EG209">
         <v>0.3045485322346502</v>
@@ -86533,7 +86533,7 @@
         <v>-2.916392425441615e-05</v>
       </c>
       <c r="EL209">
-        <v>-0.2945348538511628</v>
+        <v>-0.1928029050177691</v>
       </c>
     </row>
     <row r="210">
@@ -86541,10 +86541,10 @@
         <v>44651</v>
       </c>
       <c r="B210">
-        <v>-2.229982722819719</v>
+        <v>-2.229344333761625</v>
       </c>
       <c r="C210">
-        <v>-3.283115980530936</v>
+        <v>-3.379268200984162</v>
       </c>
       <c r="D210">
         <v>0.09128329110031413</v>
@@ -86553,10 +86553,10 @@
         <v>-0.6981285203870229</v>
       </c>
       <c r="F210">
-        <v>-1.62313749353301</v>
+        <v>-1.622499104474916</v>
       </c>
       <c r="G210">
-        <v>-0.212801630866032</v>
+        <v>-0.2121632418079379</v>
       </c>
       <c r="I210">
         <v>23157.62470023502</v>
@@ -86916,28 +86916,28 @@
         <v>-5.4673544739914</v>
       </c>
       <c r="DY210">
-        <v>-12.19825201463075</v>
+        <v>-12.16165816625504</v>
       </c>
       <c r="DZ210">
-        <v>-12.19663627990837</v>
+        <v>-12.16004243153266</v>
       </c>
       <c r="EA210">
         <v>-0.001615734722370344</v>
       </c>
       <c r="EB210">
-        <v>-93.04176908764558</v>
+        <v>-93.00517523926986</v>
       </c>
       <c r="EC210">
         <v>-5.550530838963037</v>
       </c>
       <c r="ED210">
-        <v>-87.48427400522823</v>
+        <v>-87.44768015685251</v>
       </c>
       <c r="EE210">
         <v>-0.09683043220346962</v>
       </c>
       <c r="EF210">
-        <v>-1.526185568318653</v>
+        <v>-1.525547179260559</v>
       </c>
       <c r="EG210">
         <v>0.4625094793793268</v>
@@ -86955,7 +86955,7 @@
         <v>-2.818690608743689e-05</v>
       </c>
       <c r="EL210">
-        <v>-0.2127734439599445</v>
+        <v>-0.2121350549018504</v>
       </c>
     </row>
     <row r="211">
@@ -86963,10 +86963,10 @@
         <v>44742</v>
       </c>
       <c r="B211">
-        <v>-2.090950840843372</v>
+        <v>-2.065769530723027</v>
       </c>
       <c r="C211">
-        <v>-2.886625941890521</v>
+        <v>-3.034217630275573</v>
       </c>
       <c r="D211">
         <v>-0.01234642567019492</v>
@@ -86975,10 +86975,10 @@
         <v>-0.0565513016082707</v>
       </c>
       <c r="F211">
-        <v>-2.022053113564906</v>
+        <v>-1.996871803444562</v>
       </c>
       <c r="G211">
-        <v>-0.2507917910917122</v>
+        <v>-0.225610480971368</v>
       </c>
       <c r="I211">
         <v>23384.06080548141</v>
@@ -87338,28 +87338,28 @@
         <v>-10.32601535764496</v>
       </c>
       <c r="DY211">
-        <v>-14.51935544000404</v>
+        <v>-13.06150711693613</v>
       </c>
       <c r="DZ211">
-        <v>-14.51783398887982</v>
+        <v>-13.05998566581192</v>
       </c>
       <c r="EA211">
         <v>-0.001521451124215599</v>
       </c>
       <c r="EB211">
-        <v>-117.0648678196945</v>
+        <v>-115.6070194966266</v>
       </c>
       <c r="EC211">
         <v>3.530525722647942</v>
       </c>
       <c r="ED211">
-        <v>-120.5953935423425</v>
+        <v>-119.1375452192746</v>
       </c>
       <c r="EE211">
         <v>0.06098251903377831</v>
       </c>
       <c r="EF211">
-        <v>-2.083035632598685</v>
+        <v>-2.057854322478341</v>
       </c>
       <c r="EG211">
         <v>0.4765104369239613</v>
@@ -87377,7 +87377,7 @@
         <v>-2.627991676884129e-05</v>
       </c>
       <c r="EL211">
-        <v>-0.2507655111749433</v>
+        <v>-0.225584201054599</v>
       </c>
     </row>
     <row r="212">
@@ -87385,10 +87385,10 @@
         <v>44834</v>
       </c>
       <c r="B212">
-        <v>-0.7347842365687172</v>
+        <v>-0.6857067034295107</v>
       </c>
       <c r="C212">
-        <v>-1.795258544062671</v>
+        <v>-1.751101248774911</v>
       </c>
       <c r="D212">
         <v>-0.07347397295048411</v>
@@ -87397,10 +87397,10 @@
         <v>-0.03349732029465677</v>
       </c>
       <c r="F212">
-        <v>-0.6278129433235763</v>
+        <v>-0.5787354101843698</v>
       </c>
       <c r="G212">
-        <v>-0.2156875061863692</v>
+        <v>-0.1666099730471628</v>
       </c>
       <c r="I212">
         <v>23620.8277944867</v>
@@ -87760,28 +87760,28 @@
         <v>-6.240402579596333</v>
       </c>
       <c r="DY212">
-        <v>-12.60912439911177</v>
+        <v>-9.740044351336184</v>
       </c>
       <c r="DZ212">
-        <v>-12.60768749948296</v>
+        <v>-9.738607451707386</v>
       </c>
       <c r="EA212">
         <v>-0.001436899628799324</v>
       </c>
       <c r="EB212">
-        <v>-36.7020401028669</v>
+        <v>-33.83296005509132</v>
       </c>
       <c r="EC212">
         <v>16.4522729912687</v>
       </c>
       <c r="ED212">
-        <v>-53.15431309413558</v>
+        <v>-50.28523304636001</v>
       </c>
       <c r="EE212">
         <v>0.2814271332618525</v>
       </c>
       <c r="EF212">
-        <v>-0.9092400765854284</v>
+        <v>-0.8601625434462221</v>
       </c>
       <c r="EG212">
         <v>0.5026162840447317</v>
@@ -87799,7 +87799,7 @@
         <v>-2.457912918978559e-05</v>
       </c>
       <c r="EL212">
-        <v>-0.2156629270571793</v>
+        <v>-0.166585393917973</v>
       </c>
     </row>
     <row r="213">
@@ -87807,10 +87807,10 @@
         <v>44926</v>
       </c>
       <c r="B213">
-        <v>-0.1824922128530471</v>
+        <v>-0.182429164226992</v>
       </c>
       <c r="C213">
-        <v>-1.309552503271213</v>
+        <v>-1.290812433035287</v>
       </c>
       <c r="D213">
         <v>-0.1261756957067537</v>
@@ -87819,10 +87819,10 @@
         <v>-0.0662501113593158</v>
       </c>
       <c r="F213">
-        <v>0.009933594213022369</v>
+        <v>0.009996642839077443</v>
       </c>
       <c r="G213">
-        <v>-0.06386781727518782</v>
+        <v>-0.06380476864913276</v>
       </c>
       <c r="I213">
         <v>23861.07355047205</v>
@@ -88182,28 +88182,28 @@
         <v>-4.737508650818535</v>
       </c>
       <c r="DY213">
-        <v>-3.771526783667387</v>
+        <v>-3.767803631820572</v>
       </c>
       <c r="DZ213">
-        <v>-3.770150931424038</v>
+        <v>-3.766427779577226</v>
       </c>
       <c r="EA213">
         <v>-0.001375852243344461</v>
       </c>
       <c r="EB213">
-        <v>0.5865992957152777</v>
+        <v>0.5903224475620923</v>
       </c>
       <c r="EC213">
         <v>25.57344592526352</v>
       </c>
       <c r="ED213">
-        <v>-24.98684662954817</v>
+        <v>-24.98312347770136</v>
       </c>
       <c r="EE213">
         <v>0.4330660406614975</v>
       </c>
       <c r="EF213">
-        <v>-0.4231324464484739</v>
+        <v>-0.4230693978224189</v>
       </c>
       <c r="EG213">
         <v>0.351439133076873</v>
@@ -88221,7 +88221,7 @@
         <v>-2.3298967425106e-05</v>
       </c>
       <c r="EL213">
-        <v>-0.06384451830776264</v>
+        <v>-0.06378146968170761</v>
       </c>
     </row>
   </sheetData>

</xml_diff>